<commit_message>
Fixed CSP and renamed adminReport to AdvisorReport
</commit_message>
<xml_diff>
--- a/data/progressReportTemp.xlsx
+++ b/data/progressReportTemp.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -406,7 +406,7 @@
         <v>technicalWritingApproved</v>
       </c>
       <c r="I1" t="str">
-        <v>backgroundPrepWorksheetApproved</v>
+        <v>backgroundApproved</v>
       </c>
       <c r="J1" t="str">
         <v>researchPlanningMeeting</v>
@@ -415,240 +415,80 @@
         <v>programProductRequirement</v>
       </c>
       <c r="L1" t="str">
-        <v>programOfStudyApproved</v>
+        <v>msProgramOfStudyApproved</v>
       </c>
       <c r="M1" t="str">
+        <v>phdProgramOfStudyApproved</v>
+      </c>
+      <c r="N1" t="str">
         <v>committeeCompApproved</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>phdProposalApproved</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>oralExamPassed</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>dissertationDefencePassed</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>dissertationSubmitted</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>notes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Create</v>
+        <v>fake</v>
       </c>
       <c r="B2" t="str">
-        <v>Test</v>
+        <v>fake</v>
       </c>
       <c r="C2" t="str">
-        <v>person, person</v>
+        <v>Test, Test</v>
       </c>
       <c r="E2" t="str">
-        <v>test, test</v>
+        <v>Test, Test</v>
       </c>
       <c r="G2" t="str">
-        <v/>
+        <v>2019-09-18</v>
+      </c>
+      <c r="H2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="I2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="J2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="K2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="N2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="O2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="P2" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>2019-09-18</v>
       </c>
       <c r="R2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>bodnar</v>
-      </c>
-      <c r="B3" t="str">
-        <v>hannah</v>
-      </c>
-      <c r="C3" t="str">
-        <v>person, person</v>
-      </c>
-      <c r="E3" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="Q3" t="str">
-        <v/>
-      </c>
-      <c r="R3" t="str">
-        <v>Note #3: Note 3 (2021-05-04)_x000d_third note!_x000d__x000d_Note #2: Note 2 (2021-04-18)_x000d_second note!_x000d__x000d_Note #1: Note 1 (2021-04-01)_x000d_first note!_x000d__x000d_</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>fake</v>
-      </c>
-      <c r="B4" t="str">
-        <v>fake</v>
-      </c>
-      <c r="C4" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="E4" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="G4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="H4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="I4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="J4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="K4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="L4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="M4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="N4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="O4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="P4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="Q4" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="R4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>report</v>
-      </c>
-      <c r="B5" t="str">
-        <v>progress</v>
-      </c>
-      <c r="C5" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="E5" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="G5" t="str">
-        <v/>
-      </c>
-      <c r="H5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="I5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="J5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="K5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="L5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="M5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="N5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="O5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="P5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="Q5" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="R5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>student</v>
-      </c>
-      <c r="B6" t="str">
-        <v>new</v>
-      </c>
-      <c r="C6" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="D6" t="str">
-        <v/>
-      </c>
-      <c r="F6" t="str">
-        <v>member, other</v>
-      </c>
-      <c r="R6" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>upload</v>
-      </c>
-      <c r="B7" t="str">
-        <v>test</v>
-      </c>
-      <c r="D7" t="str">
-        <v>test, test</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Pozefsky, Diane</v>
-      </c>
-      <c r="G7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="H7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="I7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="J7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="K7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="L7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="M7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="N7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="O7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="P7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="Q7" t="str">
-        <v>2019-09-18</v>
-      </c>
-      <c r="R7" t="str">
+        <v>2019-09-18</v>
+      </c>
+      <c r="S2" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>